<commit_message>
Added MLS to SPIS Use Case; TICC-410
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - SPIS Use Case v9.4.xlsx
+++ b/work-in-progress/Peppol Code Lists - SPIS Use Case v9.4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philip/dev/git-peppol/edec-codelists/work-in-progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655E8C73-4C53-F743-8444-3C4725BB718B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8491683F-E5B9-8C47-810A-F4EAD8ABA3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25420" yWindow="10340" windowWidth="11560" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>State</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>Use Case ID</t>
+  </si>
+  <si>
+    <t>MLS</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>TICC-410</t>
   </si>
 </sst>
 </file>
@@ -98,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -115,6 +127,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -522,11 +537,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -560,6 +575,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>